<commit_message>
mediciones RPL y powertrace
</commit_message>
<xml_diff>
--- a/BayesClassification/results_powertrace_wind/powertrace_wind_25_int_0_v2.xlsx
+++ b/BayesClassification/results_powertrace_wind/powertrace_wind_25_int_0_v2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -761,6 +761,153 @@
   </si>
   <si>
     <t xml:space="preserve">2018-08-30 18:27:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:28:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:28:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:28:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:28:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:28:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:28:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:29:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:29:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:29:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:29:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:29:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:29:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:30:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:30:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:30:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:30:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:30:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:30:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:31:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:31:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:31:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:31:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:31:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:31:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:32:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:32:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:32:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:32:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:32:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:32:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:33:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:33:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:33:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:33:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:33:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:33:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:34:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:34:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:34:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:34:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:34:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:34:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:35:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:35:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:35:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:35:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:35:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:35:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-30 18:36:03</t>
   </si>
 </sst>
 </file>
@@ -861,7 +1008,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q231"/>
+  <dimension ref="A1:Q280"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -13132,6 +13279,2603 @@
         <v>246</v>
       </c>
     </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="n">
+        <v>5349</v>
+      </c>
+      <c r="B232" s="0" t="n">
+        <v>295750</v>
+      </c>
+      <c r="C232" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D232" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="E232" s="0" t="n">
+        <v>7029165</v>
+      </c>
+      <c r="F232" s="0" t="n">
+        <v>68664746</v>
+      </c>
+      <c r="G232" s="0" t="n">
+        <v>3492997</v>
+      </c>
+      <c r="H232" s="0" t="n">
+        <v>1408796</v>
+      </c>
+      <c r="I232" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J232" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K232" s="0" t="n">
+        <v>37225</v>
+      </c>
+      <c r="L232" s="0" t="n">
+        <v>290455</v>
+      </c>
+      <c r="M232" s="0" t="n">
+        <v>14094</v>
+      </c>
+      <c r="N232" s="0" t="n">
+        <v>5899</v>
+      </c>
+      <c r="O232" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P232" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q232" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="n">
+        <v>5350</v>
+      </c>
+      <c r="B233" s="0" t="n">
+        <v>297030</v>
+      </c>
+      <c r="C233" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D233" s="0" t="n">
+        <v>231</v>
+      </c>
+      <c r="E233" s="0" t="n">
+        <v>7051998</v>
+      </c>
+      <c r="F233" s="0" t="n">
+        <v>68969594</v>
+      </c>
+      <c r="G233" s="0" t="n">
+        <v>3506627</v>
+      </c>
+      <c r="H233" s="0" t="n">
+        <v>1414501</v>
+      </c>
+      <c r="I233" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J233" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K233" s="0" t="n">
+        <v>22833</v>
+      </c>
+      <c r="L233" s="0" t="n">
+        <v>304848</v>
+      </c>
+      <c r="M233" s="0" t="n">
+        <v>13630</v>
+      </c>
+      <c r="N233" s="0" t="n">
+        <v>5705</v>
+      </c>
+      <c r="O233" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P233" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q233" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="n">
+        <v>5351</v>
+      </c>
+      <c r="B234" s="0" t="n">
+        <v>298310</v>
+      </c>
+      <c r="C234" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D234" s="0" t="n">
+        <v>232</v>
+      </c>
+      <c r="E234" s="0" t="n">
+        <v>7087823</v>
+      </c>
+      <c r="F234" s="0" t="n">
+        <v>69261448</v>
+      </c>
+      <c r="G234" s="0" t="n">
+        <v>3519735</v>
+      </c>
+      <c r="H234" s="0" t="n">
+        <v>1420089</v>
+      </c>
+      <c r="I234" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J234" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K234" s="0" t="n">
+        <v>35825</v>
+      </c>
+      <c r="L234" s="0" t="n">
+        <v>291854</v>
+      </c>
+      <c r="M234" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N234" s="0" t="n">
+        <v>5588</v>
+      </c>
+      <c r="O234" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P234" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q234" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="n">
+        <v>5352</v>
+      </c>
+      <c r="B235" s="0" t="n">
+        <v>299590</v>
+      </c>
+      <c r="C235" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D235" s="0" t="n">
+        <v>233</v>
+      </c>
+      <c r="E235" s="0" t="n">
+        <v>7110295</v>
+      </c>
+      <c r="F235" s="0" t="n">
+        <v>69566656</v>
+      </c>
+      <c r="G235" s="0" t="n">
+        <v>3533075</v>
+      </c>
+      <c r="H235" s="0" t="n">
+        <v>1425730</v>
+      </c>
+      <c r="I235" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J235" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K235" s="0" t="n">
+        <v>22472</v>
+      </c>
+      <c r="L235" s="0" t="n">
+        <v>305208</v>
+      </c>
+      <c r="M235" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N235" s="0" t="n">
+        <v>5641</v>
+      </c>
+      <c r="O235" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P235" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q235" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="n">
+        <v>5353</v>
+      </c>
+      <c r="B236" s="0" t="n">
+        <v>300870</v>
+      </c>
+      <c r="C236" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D236" s="0" t="n">
+        <v>234</v>
+      </c>
+      <c r="E236" s="0" t="n">
+        <v>7132771</v>
+      </c>
+      <c r="F236" s="0" t="n">
+        <v>69871860</v>
+      </c>
+      <c r="G236" s="0" t="n">
+        <v>3546415</v>
+      </c>
+      <c r="H236" s="0" t="n">
+        <v>1431371</v>
+      </c>
+      <c r="I236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K236" s="0" t="n">
+        <v>22476</v>
+      </c>
+      <c r="L236" s="0" t="n">
+        <v>305204</v>
+      </c>
+      <c r="M236" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N236" s="0" t="n">
+        <v>5641</v>
+      </c>
+      <c r="O236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P236" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q236" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="n">
+        <v>5354</v>
+      </c>
+      <c r="B237" s="0" t="n">
+        <v>302150</v>
+      </c>
+      <c r="C237" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D237" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="E237" s="0" t="n">
+        <v>7168574</v>
+      </c>
+      <c r="F237" s="0" t="n">
+        <v>70163737</v>
+      </c>
+      <c r="G237" s="0" t="n">
+        <v>3559523</v>
+      </c>
+      <c r="H237" s="0" t="n">
+        <v>1437058</v>
+      </c>
+      <c r="I237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K237" s="0" t="n">
+        <v>35803</v>
+      </c>
+      <c r="L237" s="0" t="n">
+        <v>291877</v>
+      </c>
+      <c r="M237" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N237" s="0" t="n">
+        <v>5687</v>
+      </c>
+      <c r="O237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P237" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q237" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="n">
+        <v>5355</v>
+      </c>
+      <c r="B238" s="0" t="n">
+        <v>303430</v>
+      </c>
+      <c r="C238" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D238" s="0" t="n">
+        <v>236</v>
+      </c>
+      <c r="E238" s="0" t="n">
+        <v>7191050</v>
+      </c>
+      <c r="F238" s="0" t="n">
+        <v>70468941</v>
+      </c>
+      <c r="G238" s="0" t="n">
+        <v>3572863</v>
+      </c>
+      <c r="H238" s="0" t="n">
+        <v>1442698</v>
+      </c>
+      <c r="I238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K238" s="0" t="n">
+        <v>22476</v>
+      </c>
+      <c r="L238" s="0" t="n">
+        <v>305204</v>
+      </c>
+      <c r="M238" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N238" s="0" t="n">
+        <v>5640</v>
+      </c>
+      <c r="O238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P238" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q238" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="n">
+        <v>5356</v>
+      </c>
+      <c r="B239" s="0" t="n">
+        <v>304710</v>
+      </c>
+      <c r="C239" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D239" s="0" t="n">
+        <v>237</v>
+      </c>
+      <c r="E239" s="0" t="n">
+        <v>7227770</v>
+      </c>
+      <c r="F239" s="0" t="n">
+        <v>70759901</v>
+      </c>
+      <c r="G239" s="0" t="n">
+        <v>3586551</v>
+      </c>
+      <c r="H239" s="0" t="n">
+        <v>1448508</v>
+      </c>
+      <c r="I239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K239" s="0" t="n">
+        <v>36720</v>
+      </c>
+      <c r="L239" s="0" t="n">
+        <v>290960</v>
+      </c>
+      <c r="M239" s="0" t="n">
+        <v>13688</v>
+      </c>
+      <c r="N239" s="0" t="n">
+        <v>5810</v>
+      </c>
+      <c r="O239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P239" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q239" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="n">
+        <v>5357</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>305990</v>
+      </c>
+      <c r="C240" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D240" s="0" t="n">
+        <v>238</v>
+      </c>
+      <c r="E240" s="0" t="n">
+        <v>7250243</v>
+      </c>
+      <c r="F240" s="0" t="n">
+        <v>71065108</v>
+      </c>
+      <c r="G240" s="0" t="n">
+        <v>3599891</v>
+      </c>
+      <c r="H240" s="0" t="n">
+        <v>1454146</v>
+      </c>
+      <c r="I240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K240" s="0" t="n">
+        <v>22473</v>
+      </c>
+      <c r="L240" s="0" t="n">
+        <v>305207</v>
+      </c>
+      <c r="M240" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N240" s="0" t="n">
+        <v>5638</v>
+      </c>
+      <c r="O240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P240" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q240" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="n">
+        <v>5358</v>
+      </c>
+      <c r="B241" s="0" t="n">
+        <v>307270</v>
+      </c>
+      <c r="C241" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D241" s="0" t="n">
+        <v>239</v>
+      </c>
+      <c r="E241" s="0" t="n">
+        <v>7272718</v>
+      </c>
+      <c r="F241" s="0" t="n">
+        <v>71370313</v>
+      </c>
+      <c r="G241" s="0" t="n">
+        <v>3613231</v>
+      </c>
+      <c r="H241" s="0" t="n">
+        <v>1459785</v>
+      </c>
+      <c r="I241" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J241" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K241" s="0" t="n">
+        <v>22475</v>
+      </c>
+      <c r="L241" s="0" t="n">
+        <v>305205</v>
+      </c>
+      <c r="M241" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N241" s="0" t="n">
+        <v>5639</v>
+      </c>
+      <c r="O241" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P241" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q241" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="n">
+        <v>5359</v>
+      </c>
+      <c r="B242" s="0" t="n">
+        <v>308550</v>
+      </c>
+      <c r="C242" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D242" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="E242" s="0" t="n">
+        <v>7308543</v>
+      </c>
+      <c r="F242" s="0" t="n">
+        <v>71662168</v>
+      </c>
+      <c r="G242" s="0" t="n">
+        <v>3626339</v>
+      </c>
+      <c r="H242" s="0" t="n">
+        <v>1465376</v>
+      </c>
+      <c r="I242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K242" s="0" t="n">
+        <v>35825</v>
+      </c>
+      <c r="L242" s="0" t="n">
+        <v>291855</v>
+      </c>
+      <c r="M242" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N242" s="0" t="n">
+        <v>5591</v>
+      </c>
+      <c r="O242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P242" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q242" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="n">
+        <v>5360</v>
+      </c>
+      <c r="B243" s="0" t="n">
+        <v>309830</v>
+      </c>
+      <c r="C243" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D243" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="E243" s="0" t="n">
+        <v>7331019</v>
+      </c>
+      <c r="F243" s="0" t="n">
+        <v>71967372</v>
+      </c>
+      <c r="G243" s="0" t="n">
+        <v>3639679</v>
+      </c>
+      <c r="H243" s="0" t="n">
+        <v>1471016</v>
+      </c>
+      <c r="I243" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J243" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K243" s="0" t="n">
+        <v>22476</v>
+      </c>
+      <c r="L243" s="0" t="n">
+        <v>305204</v>
+      </c>
+      <c r="M243" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N243" s="0" t="n">
+        <v>5640</v>
+      </c>
+      <c r="O243" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P243" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q243" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="n">
+        <v>5361</v>
+      </c>
+      <c r="B244" s="0" t="n">
+        <v>311110</v>
+      </c>
+      <c r="C244" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D244" s="0" t="n">
+        <v>242</v>
+      </c>
+      <c r="E244" s="0" t="n">
+        <v>7366840</v>
+      </c>
+      <c r="F244" s="0" t="n">
+        <v>72259231</v>
+      </c>
+      <c r="G244" s="0" t="n">
+        <v>3652787</v>
+      </c>
+      <c r="H244" s="0" t="n">
+        <v>1476607</v>
+      </c>
+      <c r="I244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K244" s="0" t="n">
+        <v>35821</v>
+      </c>
+      <c r="L244" s="0" t="n">
+        <v>291859</v>
+      </c>
+      <c r="M244" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N244" s="0" t="n">
+        <v>5591</v>
+      </c>
+      <c r="O244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q244" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="n">
+        <v>5362</v>
+      </c>
+      <c r="B245" s="0" t="n">
+        <v>312390</v>
+      </c>
+      <c r="C245" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D245" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="E245" s="0" t="n">
+        <v>7390135</v>
+      </c>
+      <c r="F245" s="0" t="n">
+        <v>72563616</v>
+      </c>
+      <c r="G245" s="0" t="n">
+        <v>3666649</v>
+      </c>
+      <c r="H245" s="0" t="n">
+        <v>1482451</v>
+      </c>
+      <c r="I245" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J245" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K245" s="0" t="n">
+        <v>23295</v>
+      </c>
+      <c r="L245" s="0" t="n">
+        <v>304385</v>
+      </c>
+      <c r="M245" s="0" t="n">
+        <v>13862</v>
+      </c>
+      <c r="N245" s="0" t="n">
+        <v>5844</v>
+      </c>
+      <c r="O245" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P245" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q245" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="n">
+        <v>5363</v>
+      </c>
+      <c r="B246" s="0" t="n">
+        <v>313670</v>
+      </c>
+      <c r="C246" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D246" s="0" t="n">
+        <v>244</v>
+      </c>
+      <c r="E246" s="0" t="n">
+        <v>7425964</v>
+      </c>
+      <c r="F246" s="0" t="n">
+        <v>72855467</v>
+      </c>
+      <c r="G246" s="0" t="n">
+        <v>3679757</v>
+      </c>
+      <c r="H246" s="0" t="n">
+        <v>1488041</v>
+      </c>
+      <c r="I246" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J246" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K246" s="0" t="n">
+        <v>35829</v>
+      </c>
+      <c r="L246" s="0" t="n">
+        <v>291851</v>
+      </c>
+      <c r="M246" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N246" s="0" t="n">
+        <v>5590</v>
+      </c>
+      <c r="O246" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P246" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q246" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="n">
+        <v>5364</v>
+      </c>
+      <c r="B247" s="0" t="n">
+        <v>314950</v>
+      </c>
+      <c r="C247" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D247" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="E247" s="0" t="n">
+        <v>7448443</v>
+      </c>
+      <c r="F247" s="0" t="n">
+        <v>73160668</v>
+      </c>
+      <c r="G247" s="0" t="n">
+        <v>3693097</v>
+      </c>
+      <c r="H247" s="0" t="n">
+        <v>1493678</v>
+      </c>
+      <c r="I247" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J247" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K247" s="0" t="n">
+        <v>22479</v>
+      </c>
+      <c r="L247" s="0" t="n">
+        <v>305201</v>
+      </c>
+      <c r="M247" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N247" s="0" t="n">
+        <v>5637</v>
+      </c>
+      <c r="O247" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P247" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q247" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="n">
+        <v>5365</v>
+      </c>
+      <c r="B248" s="0" t="n">
+        <v>316230</v>
+      </c>
+      <c r="C248" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D248" s="0" t="n">
+        <v>246</v>
+      </c>
+      <c r="E248" s="0" t="n">
+        <v>7483072</v>
+      </c>
+      <c r="F248" s="0" t="n">
+        <v>73453719</v>
+      </c>
+      <c r="G248" s="0" t="n">
+        <v>3716007</v>
+      </c>
+      <c r="H248" s="0" t="n">
+        <v>1501626</v>
+      </c>
+      <c r="I248" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J248" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K248" s="0" t="n">
+        <v>34629</v>
+      </c>
+      <c r="L248" s="0" t="n">
+        <v>293051</v>
+      </c>
+      <c r="M248" s="0" t="n">
+        <v>22910</v>
+      </c>
+      <c r="N248" s="0" t="n">
+        <v>7948</v>
+      </c>
+      <c r="O248" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P248" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q248" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="n">
+        <v>5366</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <v>317510</v>
+      </c>
+      <c r="C249" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D249" s="0" t="n">
+        <v>247</v>
+      </c>
+      <c r="E249" s="0" t="n">
+        <v>7518892</v>
+      </c>
+      <c r="F249" s="0" t="n">
+        <v>73745579</v>
+      </c>
+      <c r="G249" s="0" t="n">
+        <v>3729115</v>
+      </c>
+      <c r="H249" s="0" t="n">
+        <v>1507217</v>
+      </c>
+      <c r="I249" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J249" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K249" s="0" t="n">
+        <v>35820</v>
+      </c>
+      <c r="L249" s="0" t="n">
+        <v>291860</v>
+      </c>
+      <c r="M249" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N249" s="0" t="n">
+        <v>5591</v>
+      </c>
+      <c r="O249" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P249" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q249" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="n">
+        <v>5367</v>
+      </c>
+      <c r="B250" s="0" t="n">
+        <v>318790</v>
+      </c>
+      <c r="C250" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D250" s="0" t="n">
+        <v>248</v>
+      </c>
+      <c r="E250" s="0" t="n">
+        <v>7542901</v>
+      </c>
+      <c r="F250" s="0" t="n">
+        <v>74049250</v>
+      </c>
+      <c r="G250" s="0" t="n">
+        <v>3743558</v>
+      </c>
+      <c r="H250" s="0" t="n">
+        <v>1513190</v>
+      </c>
+      <c r="I250" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J250" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K250" s="0" t="n">
+        <v>24009</v>
+      </c>
+      <c r="L250" s="0" t="n">
+        <v>303671</v>
+      </c>
+      <c r="M250" s="0" t="n">
+        <v>14443</v>
+      </c>
+      <c r="N250" s="0" t="n">
+        <v>5973</v>
+      </c>
+      <c r="O250" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P250" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q250" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="n">
+        <v>5368</v>
+      </c>
+      <c r="B251" s="0" t="n">
+        <v>320070</v>
+      </c>
+      <c r="C251" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D251" s="0" t="n">
+        <v>249</v>
+      </c>
+      <c r="E251" s="0" t="n">
+        <v>7578727</v>
+      </c>
+      <c r="F251" s="0" t="n">
+        <v>74341104</v>
+      </c>
+      <c r="G251" s="0" t="n">
+        <v>3756666</v>
+      </c>
+      <c r="H251" s="0" t="n">
+        <v>1518781</v>
+      </c>
+      <c r="I251" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J251" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K251" s="0" t="n">
+        <v>35826</v>
+      </c>
+      <c r="L251" s="0" t="n">
+        <v>291854</v>
+      </c>
+      <c r="M251" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N251" s="0" t="n">
+        <v>5591</v>
+      </c>
+      <c r="O251" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P251" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q251" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="n">
+        <v>5369</v>
+      </c>
+      <c r="B252" s="0" t="n">
+        <v>321350</v>
+      </c>
+      <c r="C252" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D252" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="E252" s="0" t="n">
+        <v>7601207</v>
+      </c>
+      <c r="F252" s="0" t="n">
+        <v>74646304</v>
+      </c>
+      <c r="G252" s="0" t="n">
+        <v>3770006</v>
+      </c>
+      <c r="H252" s="0" t="n">
+        <v>1524419</v>
+      </c>
+      <c r="I252" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J252" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K252" s="0" t="n">
+        <v>22480</v>
+      </c>
+      <c r="L252" s="0" t="n">
+        <v>305200</v>
+      </c>
+      <c r="M252" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N252" s="0" t="n">
+        <v>5638</v>
+      </c>
+      <c r="O252" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P252" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q252" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="n">
+        <v>5370</v>
+      </c>
+      <c r="B253" s="0" t="n">
+        <v>322630</v>
+      </c>
+      <c r="C253" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D253" s="0" t="n">
+        <v>251</v>
+      </c>
+      <c r="E253" s="0" t="n">
+        <v>7623679</v>
+      </c>
+      <c r="F253" s="0" t="n">
+        <v>74951512</v>
+      </c>
+      <c r="G253" s="0" t="n">
+        <v>3783346</v>
+      </c>
+      <c r="H253" s="0" t="n">
+        <v>1530056</v>
+      </c>
+      <c r="I253" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J253" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K253" s="0" t="n">
+        <v>22472</v>
+      </c>
+      <c r="L253" s="0" t="n">
+        <v>305208</v>
+      </c>
+      <c r="M253" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N253" s="0" t="n">
+        <v>5637</v>
+      </c>
+      <c r="O253" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P253" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q253" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="n">
+        <v>5371</v>
+      </c>
+      <c r="B254" s="0" t="n">
+        <v>323910</v>
+      </c>
+      <c r="C254" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D254" s="0" t="n">
+        <v>252</v>
+      </c>
+      <c r="E254" s="0" t="n">
+        <v>7660185</v>
+      </c>
+      <c r="F254" s="0" t="n">
+        <v>75242686</v>
+      </c>
+      <c r="G254" s="0" t="n">
+        <v>3796860</v>
+      </c>
+      <c r="H254" s="0" t="n">
+        <v>1535826</v>
+      </c>
+      <c r="I254" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J254" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K254" s="0" t="n">
+        <v>36506</v>
+      </c>
+      <c r="L254" s="0" t="n">
+        <v>291174</v>
+      </c>
+      <c r="M254" s="0" t="n">
+        <v>13514</v>
+      </c>
+      <c r="N254" s="0" t="n">
+        <v>5770</v>
+      </c>
+      <c r="O254" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P254" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q254" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="n">
+        <v>5372</v>
+      </c>
+      <c r="B255" s="0" t="n">
+        <v>325190</v>
+      </c>
+      <c r="C255" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D255" s="0" t="n">
+        <v>253</v>
+      </c>
+      <c r="E255" s="0" t="n">
+        <v>7682660</v>
+      </c>
+      <c r="F255" s="0" t="n">
+        <v>75547891</v>
+      </c>
+      <c r="G255" s="0" t="n">
+        <v>3810200</v>
+      </c>
+      <c r="H255" s="0" t="n">
+        <v>1541469</v>
+      </c>
+      <c r="I255" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J255" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K255" s="0" t="n">
+        <v>22475</v>
+      </c>
+      <c r="L255" s="0" t="n">
+        <v>305205</v>
+      </c>
+      <c r="M255" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N255" s="0" t="n">
+        <v>5643</v>
+      </c>
+      <c r="O255" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P255" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q255" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="n">
+        <v>5373</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>326470</v>
+      </c>
+      <c r="C256" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D256" s="0" t="n">
+        <v>254</v>
+      </c>
+      <c r="E256" s="0" t="n">
+        <v>7718493</v>
+      </c>
+      <c r="F256" s="0" t="n">
+        <v>75839738</v>
+      </c>
+      <c r="G256" s="0" t="n">
+        <v>3823308</v>
+      </c>
+      <c r="H256" s="0" t="n">
+        <v>1547060</v>
+      </c>
+      <c r="I256" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J256" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K256" s="0" t="n">
+        <v>35833</v>
+      </c>
+      <c r="L256" s="0" t="n">
+        <v>291847</v>
+      </c>
+      <c r="M256" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N256" s="0" t="n">
+        <v>5591</v>
+      </c>
+      <c r="O256" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P256" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q256" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="n">
+        <v>5374</v>
+      </c>
+      <c r="B257" s="0" t="n">
+        <v>327750</v>
+      </c>
+      <c r="C257" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D257" s="0" t="n">
+        <v>255</v>
+      </c>
+      <c r="E257" s="0" t="n">
+        <v>7740966</v>
+      </c>
+      <c r="F257" s="0" t="n">
+        <v>76144945</v>
+      </c>
+      <c r="G257" s="0" t="n">
+        <v>3836648</v>
+      </c>
+      <c r="H257" s="0" t="n">
+        <v>1552699</v>
+      </c>
+      <c r="I257" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J257" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K257" s="0" t="n">
+        <v>22473</v>
+      </c>
+      <c r="L257" s="0" t="n">
+        <v>305207</v>
+      </c>
+      <c r="M257" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N257" s="0" t="n">
+        <v>5639</v>
+      </c>
+      <c r="O257" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P257" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q257" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="n">
+        <v>5375</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>329030</v>
+      </c>
+      <c r="C258" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D258" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="E258" s="0" t="n">
+        <v>7776791</v>
+      </c>
+      <c r="F258" s="0" t="n">
+        <v>76436800</v>
+      </c>
+      <c r="G258" s="0" t="n">
+        <v>3849756</v>
+      </c>
+      <c r="H258" s="0" t="n">
+        <v>1558395</v>
+      </c>
+      <c r="I258" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J258" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K258" s="0" t="n">
+        <v>35825</v>
+      </c>
+      <c r="L258" s="0" t="n">
+        <v>291855</v>
+      </c>
+      <c r="M258" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N258" s="0" t="n">
+        <v>5696</v>
+      </c>
+      <c r="O258" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P258" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q258" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="n">
+        <v>5376</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>330310</v>
+      </c>
+      <c r="C259" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D259" s="0" t="n">
+        <v>257</v>
+      </c>
+      <c r="E259" s="0" t="n">
+        <v>7799265</v>
+      </c>
+      <c r="F259" s="0" t="n">
+        <v>76742006</v>
+      </c>
+      <c r="G259" s="0" t="n">
+        <v>3863096</v>
+      </c>
+      <c r="H259" s="0" t="n">
+        <v>1564035</v>
+      </c>
+      <c r="I259" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J259" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K259" s="0" t="n">
+        <v>22473</v>
+      </c>
+      <c r="L259" s="0" t="n">
+        <v>305206</v>
+      </c>
+      <c r="M259" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N259" s="0" t="n">
+        <v>5640</v>
+      </c>
+      <c r="O259" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P259" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q259" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="n">
+        <v>5377</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>331590</v>
+      </c>
+      <c r="C260" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D260" s="0" t="n">
+        <v>258</v>
+      </c>
+      <c r="E260" s="0" t="n">
+        <v>7822275</v>
+      </c>
+      <c r="F260" s="0" t="n">
+        <v>77046676</v>
+      </c>
+      <c r="G260" s="0" t="n">
+        <v>3876726</v>
+      </c>
+      <c r="H260" s="0" t="n">
+        <v>1569935</v>
+      </c>
+      <c r="I260" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J260" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K260" s="0" t="n">
+        <v>23010</v>
+      </c>
+      <c r="L260" s="0" t="n">
+        <v>304670</v>
+      </c>
+      <c r="M260" s="0" t="n">
+        <v>13630</v>
+      </c>
+      <c r="N260" s="0" t="n">
+        <v>5900</v>
+      </c>
+      <c r="O260" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P260" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q260" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="n">
+        <v>5378</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>332870</v>
+      </c>
+      <c r="C261" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D261" s="0" t="n">
+        <v>259</v>
+      </c>
+      <c r="E261" s="0" t="n">
+        <v>7858106</v>
+      </c>
+      <c r="F261" s="0" t="n">
+        <v>77338525</v>
+      </c>
+      <c r="G261" s="0" t="n">
+        <v>3889834</v>
+      </c>
+      <c r="H261" s="0" t="n">
+        <v>1575525</v>
+      </c>
+      <c r="I261" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J261" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K261" s="0" t="n">
+        <v>35831</v>
+      </c>
+      <c r="L261" s="0" t="n">
+        <v>291849</v>
+      </c>
+      <c r="M261" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N261" s="0" t="n">
+        <v>5590</v>
+      </c>
+      <c r="O261" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P261" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q261" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="n">
+        <v>5379</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>334150</v>
+      </c>
+      <c r="C262" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D262" s="0" t="n">
+        <v>260</v>
+      </c>
+      <c r="E262" s="0" t="n">
+        <v>7882116</v>
+      </c>
+      <c r="F262" s="0" t="n">
+        <v>77642195</v>
+      </c>
+      <c r="G262" s="0" t="n">
+        <v>3904276</v>
+      </c>
+      <c r="H262" s="0" t="n">
+        <v>1581497</v>
+      </c>
+      <c r="I262" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J262" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K262" s="0" t="n">
+        <v>24010</v>
+      </c>
+      <c r="L262" s="0" t="n">
+        <v>303670</v>
+      </c>
+      <c r="M262" s="0" t="n">
+        <v>14442</v>
+      </c>
+      <c r="N262" s="0" t="n">
+        <v>5972</v>
+      </c>
+      <c r="O262" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P262" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q262" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A263" s="0" t="n">
+        <v>5380</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>335430</v>
+      </c>
+      <c r="C263" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D263" s="0" t="n">
+        <v>261</v>
+      </c>
+      <c r="E263" s="0" t="n">
+        <v>7917949</v>
+      </c>
+      <c r="F263" s="0" t="n">
+        <v>77934042</v>
+      </c>
+      <c r="G263" s="0" t="n">
+        <v>3917384</v>
+      </c>
+      <c r="H263" s="0" t="n">
+        <v>1587088</v>
+      </c>
+      <c r="I263" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J263" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K263" s="0" t="n">
+        <v>35833</v>
+      </c>
+      <c r="L263" s="0" t="n">
+        <v>291847</v>
+      </c>
+      <c r="M263" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N263" s="0" t="n">
+        <v>5591</v>
+      </c>
+      <c r="O263" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P263" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q263" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="n">
+        <v>5381</v>
+      </c>
+      <c r="B264" s="0" t="n">
+        <v>336710</v>
+      </c>
+      <c r="C264" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D264" s="0" t="n">
+        <v>262</v>
+      </c>
+      <c r="E264" s="0" t="n">
+        <v>7940424</v>
+      </c>
+      <c r="F264" s="0" t="n">
+        <v>78239247</v>
+      </c>
+      <c r="G264" s="0" t="n">
+        <v>3930724</v>
+      </c>
+      <c r="H264" s="0" t="n">
+        <v>1592725</v>
+      </c>
+      <c r="I264" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J264" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K264" s="0" t="n">
+        <v>22475</v>
+      </c>
+      <c r="L264" s="0" t="n">
+        <v>305205</v>
+      </c>
+      <c r="M264" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N264" s="0" t="n">
+        <v>5637</v>
+      </c>
+      <c r="O264" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P264" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q264" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="n">
+        <v>5382</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>337990</v>
+      </c>
+      <c r="C265" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D265" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="E265" s="0" t="n">
+        <v>7962900</v>
+      </c>
+      <c r="F265" s="0" t="n">
+        <v>78544451</v>
+      </c>
+      <c r="G265" s="0" t="n">
+        <v>3944064</v>
+      </c>
+      <c r="H265" s="0" t="n">
+        <v>1598364</v>
+      </c>
+      <c r="I265" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J265" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K265" s="0" t="n">
+        <v>22476</v>
+      </c>
+      <c r="L265" s="0" t="n">
+        <v>305204</v>
+      </c>
+      <c r="M265" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N265" s="0" t="n">
+        <v>5639</v>
+      </c>
+      <c r="O265" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P265" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q265" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="n">
+        <v>5383</v>
+      </c>
+      <c r="B266" s="0" t="n">
+        <v>339270</v>
+      </c>
+      <c r="C266" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D266" s="0" t="n">
+        <v>264</v>
+      </c>
+      <c r="E266" s="0" t="n">
+        <v>8002879</v>
+      </c>
+      <c r="F266" s="0" t="n">
+        <v>78832152</v>
+      </c>
+      <c r="G266" s="0" t="n">
+        <v>3960420</v>
+      </c>
+      <c r="H266" s="0" t="n">
+        <v>1604757</v>
+      </c>
+      <c r="I266" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J266" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K266" s="0" t="n">
+        <v>39979</v>
+      </c>
+      <c r="L266" s="0" t="n">
+        <v>287701</v>
+      </c>
+      <c r="M266" s="0" t="n">
+        <v>16356</v>
+      </c>
+      <c r="N266" s="0" t="n">
+        <v>6393</v>
+      </c>
+      <c r="O266" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P266" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q266" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="n">
+        <v>5384</v>
+      </c>
+      <c r="B267" s="0" t="n">
+        <v>340550</v>
+      </c>
+      <c r="C267" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D267" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="E267" s="0" t="n">
+        <v>8025359</v>
+      </c>
+      <c r="F267" s="0" t="n">
+        <v>79137352</v>
+      </c>
+      <c r="G267" s="0" t="n">
+        <v>3973760</v>
+      </c>
+      <c r="H267" s="0" t="n">
+        <v>1610396</v>
+      </c>
+      <c r="I267" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J267" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K267" s="0" t="n">
+        <v>22480</v>
+      </c>
+      <c r="L267" s="0" t="n">
+        <v>305200</v>
+      </c>
+      <c r="M267" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N267" s="0" t="n">
+        <v>5639</v>
+      </c>
+      <c r="O267" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P267" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q267" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A268" s="0" t="n">
+        <v>5385</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>341830</v>
+      </c>
+      <c r="C268" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D268" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="E268" s="0" t="n">
+        <v>8062506</v>
+      </c>
+      <c r="F268" s="0" t="n">
+        <v>79427885</v>
+      </c>
+      <c r="G268" s="0" t="n">
+        <v>3987796</v>
+      </c>
+      <c r="H268" s="0" t="n">
+        <v>1616280</v>
+      </c>
+      <c r="I268" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J268" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K268" s="0" t="n">
+        <v>37147</v>
+      </c>
+      <c r="L268" s="0" t="n">
+        <v>290533</v>
+      </c>
+      <c r="M268" s="0" t="n">
+        <v>14036</v>
+      </c>
+      <c r="N268" s="0" t="n">
+        <v>5884</v>
+      </c>
+      <c r="O268" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P268" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q268" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="n">
+        <v>5386</v>
+      </c>
+      <c r="B269" s="0" t="n">
+        <v>343110</v>
+      </c>
+      <c r="C269" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D269" s="0" t="n">
+        <v>267</v>
+      </c>
+      <c r="E269" s="0" t="n">
+        <v>8084979</v>
+      </c>
+      <c r="F269" s="0" t="n">
+        <v>79733092</v>
+      </c>
+      <c r="G269" s="0" t="n">
+        <v>4001136</v>
+      </c>
+      <c r="H269" s="0" t="n">
+        <v>1621919</v>
+      </c>
+      <c r="I269" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J269" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K269" s="0" t="n">
+        <v>22473</v>
+      </c>
+      <c r="L269" s="0" t="n">
+        <v>305207</v>
+      </c>
+      <c r="M269" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N269" s="0" t="n">
+        <v>5639</v>
+      </c>
+      <c r="O269" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P269" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q269" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="n">
+        <v>5387</v>
+      </c>
+      <c r="B270" s="0" t="n">
+        <v>344390</v>
+      </c>
+      <c r="C270" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D270" s="0" t="n">
+        <v>268</v>
+      </c>
+      <c r="E270" s="0" t="n">
+        <v>8120804</v>
+      </c>
+      <c r="F270" s="0" t="n">
+        <v>80024947</v>
+      </c>
+      <c r="G270" s="0" t="n">
+        <v>4014244</v>
+      </c>
+      <c r="H270" s="0" t="n">
+        <v>1627508</v>
+      </c>
+      <c r="I270" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J270" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K270" s="0" t="n">
+        <v>35825</v>
+      </c>
+      <c r="L270" s="0" t="n">
+        <v>291855</v>
+      </c>
+      <c r="M270" s="0" t="n">
+        <v>13108</v>
+      </c>
+      <c r="N270" s="0" t="n">
+        <v>5589</v>
+      </c>
+      <c r="O270" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P270" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q270" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="n">
+        <v>5388</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>345670</v>
+      </c>
+      <c r="C271" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D271" s="0" t="n">
+        <v>269</v>
+      </c>
+      <c r="E271" s="0" t="n">
+        <v>8143281</v>
+      </c>
+      <c r="F271" s="0" t="n">
+        <v>80330150</v>
+      </c>
+      <c r="G271" s="0" t="n">
+        <v>4027584</v>
+      </c>
+      <c r="H271" s="0" t="n">
+        <v>1633147</v>
+      </c>
+      <c r="I271" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J271" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K271" s="0" t="n">
+        <v>22477</v>
+      </c>
+      <c r="L271" s="0" t="n">
+        <v>305203</v>
+      </c>
+      <c r="M271" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N271" s="0" t="n">
+        <v>5639</v>
+      </c>
+      <c r="O271" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P271" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q271" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="n">
+        <v>5389</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>346950</v>
+      </c>
+      <c r="C272" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D272" s="0" t="n">
+        <v>270</v>
+      </c>
+      <c r="E272" s="0" t="n">
+        <v>8165752</v>
+      </c>
+      <c r="F272" s="0" t="n">
+        <v>80635359</v>
+      </c>
+      <c r="G272" s="0" t="n">
+        <v>4040924</v>
+      </c>
+      <c r="H272" s="0" t="n">
+        <v>1638788</v>
+      </c>
+      <c r="I272" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J272" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K272" s="0" t="n">
+        <v>22471</v>
+      </c>
+      <c r="L272" s="0" t="n">
+        <v>305209</v>
+      </c>
+      <c r="M272" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N272" s="0" t="n">
+        <v>5641</v>
+      </c>
+      <c r="O272" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P272" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q272" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A273" s="0" t="n">
+        <v>5390</v>
+      </c>
+      <c r="B273" s="0" t="n">
+        <v>348230</v>
+      </c>
+      <c r="C273" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D273" s="0" t="n">
+        <v>271</v>
+      </c>
+      <c r="E273" s="0" t="n">
+        <v>8221436</v>
+      </c>
+      <c r="F273" s="0" t="n">
+        <v>80907355</v>
+      </c>
+      <c r="G273" s="0" t="n">
+        <v>4069518</v>
+      </c>
+      <c r="H273" s="0" t="n">
+        <v>1648183</v>
+      </c>
+      <c r="I273" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J273" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K273" s="0" t="n">
+        <v>55684</v>
+      </c>
+      <c r="L273" s="0" t="n">
+        <v>271996</v>
+      </c>
+      <c r="M273" s="0" t="n">
+        <v>28594</v>
+      </c>
+      <c r="N273" s="0" t="n">
+        <v>9395</v>
+      </c>
+      <c r="O273" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P273" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q273" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="n">
+        <v>5391</v>
+      </c>
+      <c r="B274" s="0" t="n">
+        <v>349510</v>
+      </c>
+      <c r="C274" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D274" s="0" t="n">
+        <v>272</v>
+      </c>
+      <c r="E274" s="0" t="n">
+        <v>8243914</v>
+      </c>
+      <c r="F274" s="0" t="n">
+        <v>81212557</v>
+      </c>
+      <c r="G274" s="0" t="n">
+        <v>4082858</v>
+      </c>
+      <c r="H274" s="0" t="n">
+        <v>1653822</v>
+      </c>
+      <c r="I274" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J274" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K274" s="0" t="n">
+        <v>22478</v>
+      </c>
+      <c r="L274" s="0" t="n">
+        <v>305202</v>
+      </c>
+      <c r="M274" s="0" t="n">
+        <v>13340</v>
+      </c>
+      <c r="N274" s="0" t="n">
+        <v>5639</v>
+      </c>
+      <c r="O274" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P274" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q274" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="n">
+        <v>5392</v>
+      </c>
+      <c r="B275" s="0" t="n">
+        <v>350790</v>
+      </c>
+      <c r="C275" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D275" s="0" t="n">
+        <v>273</v>
+      </c>
+      <c r="E275" s="0" t="n">
+        <v>8279701</v>
+      </c>
+      <c r="F275" s="0" t="n">
+        <v>81504450</v>
+      </c>
+      <c r="G275" s="0" t="n">
+        <v>4095908</v>
+      </c>
+      <c r="H275" s="0" t="n">
+        <v>1659401</v>
+      </c>
+      <c r="I275" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J275" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K275" s="0" t="n">
+        <v>35787</v>
+      </c>
+      <c r="L275" s="0" t="n">
+        <v>291893</v>
+      </c>
+      <c r="M275" s="0" t="n">
+        <v>13050</v>
+      </c>
+      <c r="N275" s="0" t="n">
+        <v>5579</v>
+      </c>
+      <c r="O275" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P275" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q275" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="n">
+        <v>5393</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>352070</v>
+      </c>
+      <c r="C276" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D276" s="0" t="n">
+        <v>274</v>
+      </c>
+      <c r="E276" s="0" t="n">
+        <v>8302142</v>
+      </c>
+      <c r="F276" s="0" t="n">
+        <v>81809689</v>
+      </c>
+      <c r="G276" s="0" t="n">
+        <v>4109190</v>
+      </c>
+      <c r="H276" s="0" t="n">
+        <v>1665223</v>
+      </c>
+      <c r="I276" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J276" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K276" s="0" t="n">
+        <v>22441</v>
+      </c>
+      <c r="L276" s="0" t="n">
+        <v>305239</v>
+      </c>
+      <c r="M276" s="0" t="n">
+        <v>13282</v>
+      </c>
+      <c r="N276" s="0" t="n">
+        <v>5822</v>
+      </c>
+      <c r="O276" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P276" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q276" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="n">
+        <v>5394</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>353350</v>
+      </c>
+      <c r="C277" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D277" s="0" t="n">
+        <v>275</v>
+      </c>
+      <c r="E277" s="0" t="n">
+        <v>8323981</v>
+      </c>
+      <c r="F277" s="0" t="n">
+        <v>82115530</v>
+      </c>
+      <c r="G277" s="0" t="n">
+        <v>4122008</v>
+      </c>
+      <c r="H277" s="0" t="n">
+        <v>1670741</v>
+      </c>
+      <c r="I277" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J277" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K277" s="0" t="n">
+        <v>21839</v>
+      </c>
+      <c r="L277" s="0" t="n">
+        <v>305841</v>
+      </c>
+      <c r="M277" s="0" t="n">
+        <v>12818</v>
+      </c>
+      <c r="N277" s="0" t="n">
+        <v>5518</v>
+      </c>
+      <c r="O277" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P277" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q277" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="n">
+        <v>5395</v>
+      </c>
+      <c r="B278" s="0" t="n">
+        <v>354630</v>
+      </c>
+      <c r="C278" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D278" s="0" t="n">
+        <v>276</v>
+      </c>
+      <c r="E278" s="0" t="n">
+        <v>8359124</v>
+      </c>
+      <c r="F278" s="0" t="n">
+        <v>82408067</v>
+      </c>
+      <c r="G278" s="0" t="n">
+        <v>4134536</v>
+      </c>
+      <c r="H278" s="0" t="n">
+        <v>1676306</v>
+      </c>
+      <c r="I278" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J278" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K278" s="0" t="n">
+        <v>35143</v>
+      </c>
+      <c r="L278" s="0" t="n">
+        <v>292537</v>
+      </c>
+      <c r="M278" s="0" t="n">
+        <v>12528</v>
+      </c>
+      <c r="N278" s="0" t="n">
+        <v>5565</v>
+      </c>
+      <c r="O278" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P278" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q278" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="0" t="n">
+        <v>5396</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>355910</v>
+      </c>
+      <c r="C279" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D279" s="0" t="n">
+        <v>277</v>
+      </c>
+      <c r="E279" s="0" t="n">
+        <v>8384154</v>
+      </c>
+      <c r="F279" s="0" t="n">
+        <v>82710717</v>
+      </c>
+      <c r="G279" s="0" t="n">
+        <v>4149558</v>
+      </c>
+      <c r="H279" s="0" t="n">
+        <v>1682568</v>
+      </c>
+      <c r="I279" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J279" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K279" s="0" t="n">
+        <v>25030</v>
+      </c>
+      <c r="L279" s="0" t="n">
+        <v>302650</v>
+      </c>
+      <c r="M279" s="0" t="n">
+        <v>15022</v>
+      </c>
+      <c r="N279" s="0" t="n">
+        <v>6262</v>
+      </c>
+      <c r="O279" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P279" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q279" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="0" t="n">
+        <v>5397</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>357190</v>
+      </c>
+      <c r="C280" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D280" s="0" t="n">
+        <v>278</v>
+      </c>
+      <c r="E280" s="0" t="n">
+        <v>8422684</v>
+      </c>
+      <c r="F280" s="0" t="n">
+        <v>82999867</v>
+      </c>
+      <c r="G280" s="0" t="n">
+        <v>4164580</v>
+      </c>
+      <c r="H280" s="0" t="n">
+        <v>1688779</v>
+      </c>
+      <c r="I280" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J280" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K280" s="0" t="n">
+        <v>38530</v>
+      </c>
+      <c r="L280" s="0" t="n">
+        <v>289150</v>
+      </c>
+      <c r="M280" s="0" t="n">
+        <v>15022</v>
+      </c>
+      <c r="N280" s="0" t="n">
+        <v>6211</v>
+      </c>
+      <c r="O280" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P280" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q280" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>